<commit_message>
added fake mds and edited mds_canon file
</commit_message>
<xml_diff>
--- a/data-raw/mdsR_dict.xlsx
+++ b/data-raw/mdsR_dict.xlsx
@@ -2034,8 +2034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G190" sqref="G190"/>
+    <sheetView tabSelected="1" topLeftCell="A190" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2085,7 +2085,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>214</v>
@@ -2108,7 +2108,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>216</v>
@@ -2131,7 +2131,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>218</v>
@@ -2154,7 +2154,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>220</v>
@@ -2177,7 +2177,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>240</v>
@@ -2200,7 +2200,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>222</v>
@@ -2223,7 +2223,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>224</v>
@@ -2246,7 +2246,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>225</v>
@@ -2269,7 +2269,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>220</v>
@@ -2292,7 +2292,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>230</v>
@@ -2315,7 +2315,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>232</v>
@@ -2338,7 +2338,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>234</v>
@@ -2361,7 +2361,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>236</v>

</xml_diff>

<commit_message>
updated documentation, website, added swallowing dz
</commit_message>
<xml_diff>
--- a/data-raw/mdsR_dict.xlsx
+++ b/data-raw/mdsR_dict.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="558">
   <si>
     <t xml:space="preserve"> accpt_id </t>
   </si>
@@ -1663,6 +1663,42 @@
   </si>
   <si>
     <t>SetMissToZero</t>
+  </si>
+  <si>
+    <t>M3K0100A</t>
+  </si>
+  <si>
+    <t>M3J1400</t>
+  </si>
+  <si>
+    <t>Prognosis - less than 6 months</t>
+  </si>
+  <si>
+    <t>M3K0100B</t>
+  </si>
+  <si>
+    <t>M3K0100C</t>
+  </si>
+  <si>
+    <t>M3K0100D</t>
+  </si>
+  <si>
+    <t>M3K0100Z</t>
+  </si>
+  <si>
+    <t>Swallowing - Loss of food when eating</t>
+  </si>
+  <si>
+    <t>Swallowing - residual in mouth</t>
+  </si>
+  <si>
+    <t>Swallowing - choking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swallowing - Pain </t>
+  </si>
+  <si>
+    <t>Swallowing - none of above</t>
   </si>
 </sst>
 </file>
@@ -2032,10 +2068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I223"/>
+  <dimension ref="A1:I229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B14"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5591,13 +5627,13 @@
     </row>
     <row r="147" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="5" t="s">
-        <v>145</v>
+        <v>547</v>
       </c>
       <c r="B147" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C147" s="6" t="s">
-        <v>480</v>
+        <v>548</v>
       </c>
       <c r="D147" s="6" t="s">
         <v>375</v>
@@ -5617,13 +5653,13 @@
     </row>
     <row r="148" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B148" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D148" s="6" t="s">
         <v>375</v>
@@ -5643,13 +5679,13 @@
     </row>
     <row r="149" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B149" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D149" s="6" t="s">
         <v>375</v>
@@ -5669,13 +5705,13 @@
     </row>
     <row r="150" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B150" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C150" s="6" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D150" s="6" t="s">
         <v>375</v>
@@ -5695,13 +5731,13 @@
     </row>
     <row r="151" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B151" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C151" s="6" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D151" s="6" t="s">
         <v>375</v>
@@ -5721,13 +5757,13 @@
     </row>
     <row r="152" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B152" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C152" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D152" s="6" t="s">
         <v>375</v>
@@ -5747,13 +5783,13 @@
     </row>
     <row r="153" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B153" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C153" s="6" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D153" s="6" t="s">
         <v>375</v>
@@ -5773,13 +5809,13 @@
     </row>
     <row r="154" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B154" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C154" s="6" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D154" s="6" t="s">
         <v>375</v>
@@ -5799,13 +5835,13 @@
     </row>
     <row r="155" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B155" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C155" s="6" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D155" s="6" t="s">
         <v>375</v>
@@ -5825,44 +5861,68 @@
     </row>
     <row r="156" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B156" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C156" s="6" t="s">
-        <v>370</v>
+        <v>488</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>372</v>
+        <v>375</v>
+      </c>
+      <c r="E156" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="F156" s="9" t="s">
+        <v>491</v>
+      </c>
+      <c r="H156" s="13" t="s">
+        <v>520</v>
+      </c>
+      <c r="I156" s="10" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="157" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="5" t="s">
-        <v>155</v>
+        <v>546</v>
       </c>
       <c r="B157" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C157" s="6" t="s">
-        <v>371</v>
+        <v>553</v>
       </c>
       <c r="D157" s="6" t="s">
-        <v>373</v>
+        <v>375</v>
+      </c>
+      <c r="E157" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="F157" s="9" t="s">
+        <v>490</v>
+      </c>
+      <c r="H157" s="13" t="s">
+        <v>520</v>
+      </c>
+      <c r="I157" s="10" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="158" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="5" t="s">
-        <v>156</v>
+        <v>549</v>
       </c>
       <c r="B158" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C158" s="6" t="s">
-        <v>489</v>
+        <v>554</v>
       </c>
       <c r="D158" s="6" t="s">
-        <v>538</v>
+        <v>375</v>
       </c>
       <c r="E158" s="11" t="s">
         <v>357</v>
@@ -5871,21 +5931,21 @@
         <v>490</v>
       </c>
       <c r="H158" s="13" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="I158" s="10" t="s">
-        <v>539</v>
+        <v>390</v>
       </c>
     </row>
     <row r="159" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="5" t="s">
-        <v>157</v>
+        <v>550</v>
       </c>
       <c r="B159" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C159" s="6" t="s">
-        <v>492</v>
+        <v>555</v>
       </c>
       <c r="D159" s="6" t="s">
         <v>375</v>
@@ -5905,13 +5965,13 @@
     </row>
     <row r="160" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="5" t="s">
-        <v>158</v>
+        <v>551</v>
       </c>
       <c r="B160" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C160" s="6" t="s">
-        <v>493</v>
+        <v>556</v>
       </c>
       <c r="D160" s="6" t="s">
         <v>375</v>
@@ -5931,13 +5991,13 @@
     </row>
     <row r="161" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="5" t="s">
-        <v>159</v>
+        <v>552</v>
       </c>
       <c r="B161" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C161" s="6" t="s">
-        <v>494</v>
+        <v>557</v>
       </c>
       <c r="D161" s="6" t="s">
         <v>375</v>
@@ -5957,91 +6017,67 @@
     </row>
     <row r="162" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="5" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B162" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C162" s="6" t="s">
-        <v>495</v>
+        <v>370</v>
       </c>
       <c r="D162" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="E162" s="11" t="s">
-        <v>357</v>
-      </c>
-      <c r="F162" s="9" t="s">
-        <v>490</v>
-      </c>
-      <c r="H162" s="13" t="s">
-        <v>520</v>
-      </c>
-      <c r="I162" s="10" t="s">
-        <v>390</v>
+        <v>372</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="5" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B163" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C163" s="6" t="s">
-        <v>496</v>
+        <v>371</v>
       </c>
       <c r="D163" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="E163" s="11" t="s">
-        <v>357</v>
-      </c>
-      <c r="F163" s="9" t="s">
-        <v>490</v>
-      </c>
-      <c r="H163" s="13" t="s">
-        <v>520</v>
-      </c>
-      <c r="I163" s="10" t="s">
-        <v>390</v>
+        <v>373</v>
       </c>
     </row>
     <row r="164" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="5" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B164" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C164" s="6" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="D164" s="6" t="s">
-        <v>375</v>
+        <v>538</v>
       </c>
       <c r="E164" s="11" t="s">
         <v>357</v>
       </c>
       <c r="F164" s="9" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="H164" s="13" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="I164" s="10" t="s">
-        <v>390</v>
+        <v>539</v>
       </c>
     </row>
     <row r="165" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="5" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B165" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C165" s="6" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="D165" s="6" t="s">
         <v>375</v>
@@ -6050,7 +6086,7 @@
         <v>357</v>
       </c>
       <c r="F165" s="9" t="s">
-        <v>500</v>
+        <v>490</v>
       </c>
       <c r="H165" s="13" t="s">
         <v>520</v>
@@ -6061,73 +6097,163 @@
     </row>
     <row r="166" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="5" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B166" s="5" t="s">
         <v>543</v>
       </c>
+      <c r="C166" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="D166" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="E166" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="F166" s="9" t="s">
+        <v>490</v>
+      </c>
       <c r="H166" s="13" t="s">
-        <v>523</v>
+        <v>520</v>
+      </c>
+      <c r="I166" s="10" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="167" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B167" s="5" t="s">
         <v>543</v>
       </c>
+      <c r="C167" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="D167" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="E167" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="F167" s="9" t="s">
+        <v>490</v>
+      </c>
       <c r="H167" s="13" t="s">
-        <v>523</v>
+        <v>520</v>
+      </c>
+      <c r="I167" s="10" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="168" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="5" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B168" s="5" t="s">
         <v>543</v>
       </c>
+      <c r="C168" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="D168" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="E168" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="F168" s="9" t="s">
+        <v>490</v>
+      </c>
       <c r="H168" s="13" t="s">
-        <v>523</v>
+        <v>520</v>
+      </c>
+      <c r="I168" s="10" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="169" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="5" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B169" s="5" t="s">
         <v>543</v>
       </c>
+      <c r="C169" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="D169" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="E169" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="F169" s="9" t="s">
+        <v>490</v>
+      </c>
       <c r="H169" s="13" t="s">
-        <v>523</v>
+        <v>520</v>
+      </c>
+      <c r="I169" s="10" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="170" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="5" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B170" s="5" t="s">
         <v>543</v>
       </c>
+      <c r="C170" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="D170" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="E170" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="F170" s="9" t="s">
+        <v>498</v>
+      </c>
       <c r="H170" s="13" t="s">
-        <v>523</v>
+        <v>520</v>
+      </c>
+      <c r="I170" s="10" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="171" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="5" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B171" s="5" t="s">
         <v>543</v>
       </c>
+      <c r="C171" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="D171" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="E171" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="F171" s="9" t="s">
+        <v>500</v>
+      </c>
       <c r="H171" s="13" t="s">
-        <v>523</v>
+        <v>520</v>
+      </c>
+      <c r="I171" s="10" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="172" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B172" s="5" t="s">
         <v>543</v>
@@ -6138,22 +6264,10 @@
     </row>
     <row r="173" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="5" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B173" s="5" t="s">
         <v>543</v>
-      </c>
-      <c r="C173" s="6" t="s">
-        <v>501</v>
-      </c>
-      <c r="D173" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="E173" s="11" t="s">
-        <v>357</v>
-      </c>
-      <c r="F173" s="9" t="s">
-        <v>500</v>
       </c>
       <c r="H173" s="13" t="s">
         <v>523</v>
@@ -6161,22 +6275,10 @@
     </row>
     <row r="174" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="5" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B174" s="5" t="s">
         <v>543</v>
-      </c>
-      <c r="C174" s="6" t="s">
-        <v>502</v>
-      </c>
-      <c r="D174" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="E174" s="11" t="s">
-        <v>357</v>
-      </c>
-      <c r="F174" s="9" t="s">
-        <v>500</v>
       </c>
       <c r="H174" s="13" t="s">
         <v>523</v>
@@ -6184,22 +6286,10 @@
     </row>
     <row r="175" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B175" s="5" t="s">
         <v>543</v>
-      </c>
-      <c r="C175" s="6" t="s">
-        <v>503</v>
-      </c>
-      <c r="D175" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="E175" s="11" t="s">
-        <v>357</v>
-      </c>
-      <c r="F175" s="9" t="s">
-        <v>500</v>
       </c>
       <c r="H175" s="13" t="s">
         <v>523</v>
@@ -6207,22 +6297,10 @@
     </row>
     <row r="176" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="5" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B176" s="5" t="s">
         <v>543</v>
-      </c>
-      <c r="C176" s="6" t="s">
-        <v>504</v>
-      </c>
-      <c r="D176" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="E176" s="11" t="s">
-        <v>357</v>
-      </c>
-      <c r="F176" s="9" t="s">
-        <v>500</v>
       </c>
       <c r="H176" s="13" t="s">
         <v>523</v>
@@ -6230,22 +6308,10 @@
     </row>
     <row r="177" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="5" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B177" s="5" t="s">
         <v>543</v>
-      </c>
-      <c r="C177" s="6" t="s">
-        <v>505</v>
-      </c>
-      <c r="D177" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="E177" s="11" t="s">
-        <v>357</v>
-      </c>
-      <c r="F177" s="9" t="s">
-        <v>500</v>
       </c>
       <c r="H177" s="13" t="s">
         <v>523</v>
@@ -6253,7 +6319,7 @@
     </row>
     <row r="178" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="5" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B178" s="5" t="s">
         <v>543</v>
@@ -6264,13 +6330,13 @@
     </row>
     <row r="179" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="5" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B179" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C179" s="6" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="D179" s="6" t="s">
         <v>375</v>
@@ -6279,27 +6345,21 @@
         <v>357</v>
       </c>
       <c r="F179" s="9" t="s">
-        <v>513</v>
-      </c>
-      <c r="G179" s="9" t="b">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="H179" s="13" t="s">
-        <v>520</v>
-      </c>
-      <c r="I179" s="10" t="s">
-        <v>540</v>
+        <v>523</v>
       </c>
     </row>
     <row r="180" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="5" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B180" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C180" s="6" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="D180" s="6" t="s">
         <v>375</v>
@@ -6308,27 +6368,21 @@
         <v>357</v>
       </c>
       <c r="F180" s="9" t="s">
-        <v>513</v>
-      </c>
-      <c r="G180" s="9" t="b">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="H180" s="13" t="s">
-        <v>520</v>
-      </c>
-      <c r="I180" s="10" t="s">
-        <v>540</v>
+        <v>523</v>
       </c>
     </row>
     <row r="181" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="5" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B181" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C181" s="6" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="D181" s="6" t="s">
         <v>375</v>
@@ -6337,27 +6391,21 @@
         <v>357</v>
       </c>
       <c r="F181" s="9" t="s">
-        <v>513</v>
-      </c>
-      <c r="G181" s="9" t="b">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="H181" s="13" t="s">
-        <v>520</v>
-      </c>
-      <c r="I181" s="10" t="s">
-        <v>540</v>
+        <v>523</v>
       </c>
     </row>
     <row r="182" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="5" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B182" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C182" s="6" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="D182" s="6" t="s">
         <v>375</v>
@@ -6366,27 +6414,21 @@
         <v>357</v>
       </c>
       <c r="F182" s="9" t="s">
-        <v>513</v>
-      </c>
-      <c r="G182" s="9" t="b">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="H182" s="13" t="s">
-        <v>520</v>
-      </c>
-      <c r="I182" s="10" t="s">
-        <v>540</v>
+        <v>523</v>
       </c>
     </row>
     <row r="183" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="5" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B183" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C183" s="6" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="D183" s="6" t="s">
         <v>375</v>
@@ -6395,56 +6437,32 @@
         <v>357</v>
       </c>
       <c r="F183" s="9" t="s">
-        <v>513</v>
-      </c>
-      <c r="G183" s="9" t="b">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="H183" s="13" t="s">
-        <v>520</v>
-      </c>
-      <c r="I183" s="10" t="s">
-        <v>540</v>
+        <v>523</v>
       </c>
     </row>
     <row r="184" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="5" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B184" s="5" t="s">
         <v>543</v>
       </c>
-      <c r="C184" s="6" t="s">
-        <v>511</v>
-      </c>
-      <c r="D184" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="E184" s="11" t="s">
-        <v>357</v>
-      </c>
-      <c r="F184" s="9" t="s">
-        <v>513</v>
-      </c>
-      <c r="G184" s="9" t="b">
-        <v>1</v>
-      </c>
       <c r="H184" s="13" t="s">
-        <v>520</v>
-      </c>
-      <c r="I184" s="10" t="s">
-        <v>540</v>
+        <v>523</v>
       </c>
     </row>
     <row r="185" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="5" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B185" s="5" t="s">
         <v>543</v>
       </c>
       <c r="C185" s="6" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="D185" s="6" t="s">
         <v>375</v>
@@ -6467,73 +6485,181 @@
     </row>
     <row r="186" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="5" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B186" s="5" t="s">
         <v>543</v>
       </c>
+      <c r="C186" s="6" t="s">
+        <v>507</v>
+      </c>
+      <c r="D186" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="E186" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="F186" s="9" t="s">
+        <v>513</v>
+      </c>
+      <c r="G186" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="H186" s="13" t="s">
-        <v>523</v>
+        <v>520</v>
+      </c>
+      <c r="I186" s="10" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="187" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="5" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B187" s="5" t="s">
         <v>543</v>
       </c>
+      <c r="C187" s="6" t="s">
+        <v>508</v>
+      </c>
+      <c r="D187" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="E187" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="F187" s="9" t="s">
+        <v>513</v>
+      </c>
+      <c r="G187" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="H187" s="13" t="s">
-        <v>523</v>
+        <v>520</v>
+      </c>
+      <c r="I187" s="10" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="188" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="5" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B188" s="5" t="s">
         <v>543</v>
       </c>
+      <c r="C188" s="6" t="s">
+        <v>509</v>
+      </c>
+      <c r="D188" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="E188" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="F188" s="9" t="s">
+        <v>513</v>
+      </c>
+      <c r="G188" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="H188" s="13" t="s">
-        <v>523</v>
+        <v>520</v>
+      </c>
+      <c r="I188" s="10" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="189" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="5" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B189" s="5" t="s">
         <v>543</v>
       </c>
+      <c r="C189" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="D189" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="E189" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="F189" s="9" t="s">
+        <v>513</v>
+      </c>
+      <c r="G189" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="H189" s="13" t="s">
-        <v>523</v>
+        <v>520</v>
+      </c>
+      <c r="I189" s="10" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="190" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="5" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B190" s="5" t="s">
         <v>543</v>
       </c>
+      <c r="C190" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="D190" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="E190" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="F190" s="9" t="s">
+        <v>513</v>
+      </c>
+      <c r="G190" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="H190" s="13" t="s">
-        <v>523</v>
+        <v>520</v>
+      </c>
+      <c r="I190" s="10" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="191" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="5" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B191" s="5" t="s">
         <v>543</v>
       </c>
+      <c r="C191" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="D191" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="E191" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="F191" s="9" t="s">
+        <v>513</v>
+      </c>
+      <c r="G191" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="H191" s="13" t="s">
-        <v>523</v>
+        <v>520</v>
+      </c>
+      <c r="I191" s="10" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="192" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" s="5" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B192" s="5" t="s">
         <v>543</v>
@@ -6542,9 +6668,9 @@
         <v>523</v>
       </c>
     </row>
-    <row r="193" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:8" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="5" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B193" s="5" t="s">
         <v>543</v>
@@ -6553,9 +6679,9 @@
         <v>523</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:8" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" s="5" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B194" s="5" t="s">
         <v>543</v>
@@ -6564,9 +6690,9 @@
         <v>523</v>
       </c>
     </row>
-    <row r="195" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:8" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B195" s="5" t="s">
         <v>543</v>
@@ -6575,9 +6701,9 @@
         <v>523</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:8" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" s="5" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B196" s="5" t="s">
         <v>543</v>
@@ -6586,9 +6712,9 @@
         <v>523</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:8" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" s="5" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B197" s="5" t="s">
         <v>543</v>
@@ -6597,9 +6723,9 @@
         <v>523</v>
       </c>
     </row>
-    <row r="198" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:8" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="5" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B198" s="5" t="s">
         <v>543</v>
@@ -6608,9 +6734,9 @@
         <v>523</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:8" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" s="5" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B199" s="5" t="s">
         <v>543</v>
@@ -6619,9 +6745,9 @@
         <v>523</v>
       </c>
     </row>
-    <row r="200" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:8" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="5" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B200" s="5" t="s">
         <v>543</v>
@@ -6630,9 +6756,9 @@
         <v>523</v>
       </c>
     </row>
-    <row r="201" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:8" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" s="5" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B201" s="5" t="s">
         <v>543</v>
@@ -6641,9 +6767,9 @@
         <v>523</v>
       </c>
     </row>
-    <row r="202" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:8" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" s="5" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B202" s="5" t="s">
         <v>543</v>
@@ -6652,9 +6778,9 @@
         <v>523</v>
       </c>
     </row>
-    <row r="203" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:8" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" s="5" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B203" s="5" t="s">
         <v>543</v>
@@ -6663,9 +6789,9 @@
         <v>523</v>
       </c>
     </row>
-    <row r="204" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:8" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" s="5" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B204" s="5" t="s">
         <v>543</v>
@@ -6674,9 +6800,9 @@
         <v>523</v>
       </c>
     </row>
-    <row r="205" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:8" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" s="5" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B205" s="5" t="s">
         <v>543</v>
@@ -6685,9 +6811,9 @@
         <v>523</v>
       </c>
     </row>
-    <row r="206" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:8" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" s="5" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B206" s="5" t="s">
         <v>543</v>
@@ -6696,127 +6822,67 @@
         <v>523</v>
       </c>
     </row>
-    <row r="207" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:8" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A207" s="5" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B207" s="5" t="s">
         <v>543</v>
       </c>
-      <c r="C207" s="6" t="s">
-        <v>376</v>
-      </c>
-      <c r="D207" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="E207" s="11" t="s">
-        <v>357</v>
-      </c>
       <c r="H207" s="13" t="s">
-        <v>520</v>
-      </c>
-      <c r="I207" s="10" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="208" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A208" s="5" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B208" s="5" t="s">
         <v>543</v>
       </c>
-      <c r="C208" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="D208" s="6" t="s">
-        <v>379</v>
-      </c>
-      <c r="E208" s="11" t="s">
-        <v>357</v>
-      </c>
       <c r="H208" s="13" t="s">
-        <v>520</v>
-      </c>
-      <c r="I208" s="10" t="s">
-        <v>390</v>
+        <v>523</v>
       </c>
     </row>
     <row r="209" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" s="5" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B209" s="5" t="s">
         <v>543</v>
       </c>
-      <c r="C209" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="D209" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="E209" s="11" t="s">
-        <v>357</v>
-      </c>
       <c r="H209" s="13" t="s">
-        <v>520</v>
-      </c>
-      <c r="I209" s="10" t="s">
-        <v>390</v>
+        <v>523</v>
       </c>
     </row>
     <row r="210" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A210" s="5" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B210" s="5" t="s">
         <v>543</v>
       </c>
-      <c r="C210" s="6" t="s">
-        <v>400</v>
-      </c>
-      <c r="D210" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="E210" s="11" t="s">
-        <v>357</v>
-      </c>
       <c r="H210" s="13" t="s">
-        <v>520</v>
-      </c>
-      <c r="I210" s="10" t="s">
-        <v>541</v>
+        <v>523</v>
       </c>
     </row>
     <row r="211" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" s="5" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B211" s="5" t="s">
         <v>543</v>
       </c>
-      <c r="C211" s="6" t="s">
-        <v>402</v>
-      </c>
-      <c r="D211" s="6" t="s">
-        <v>403</v>
-      </c>
-      <c r="E211" s="11" t="s">
-        <v>357</v>
-      </c>
       <c r="H211" s="13" t="s">
-        <v>520</v>
-      </c>
-      <c r="I211" s="10" t="s">
-        <v>404</v>
+        <v>523</v>
       </c>
     </row>
     <row r="212" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" s="5" t="s">
-        <v>9</v>
+        <v>204</v>
       </c>
       <c r="B212" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H212" s="13" t="s">
         <v>523</v>
@@ -6824,164 +6890,290 @@
     </row>
     <row r="213" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" s="5" t="s">
-        <v>10</v>
+        <v>205</v>
       </c>
       <c r="B213" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
+      </c>
+      <c r="C213" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="D213" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="E213" s="11" t="s">
+        <v>357</v>
       </c>
       <c r="H213" s="13" t="s">
-        <v>523</v>
+        <v>520</v>
+      </c>
+      <c r="I213" s="10" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="214" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" s="5" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B214" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
+      </c>
+      <c r="C214" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="D214" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="E214" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="H214" s="13" t="s">
+        <v>520</v>
+      </c>
+      <c r="I214" s="10" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="215" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A215" s="5" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B215" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
+      </c>
+      <c r="C215" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="D215" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="E215" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="H215" s="13" t="s">
+        <v>520</v>
+      </c>
+      <c r="I215" s="10" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="216" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" s="5" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B216" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
+      </c>
+      <c r="C216" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="D216" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="E216" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="H216" s="13" t="s">
+        <v>520</v>
+      </c>
+      <c r="I216" s="10" t="s">
+        <v>541</v>
       </c>
     </row>
     <row r="217" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B217" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
+      </c>
+      <c r="C217" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="D217" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="E217" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="H217" s="13" t="s">
+        <v>520</v>
+      </c>
+      <c r="I217" s="10" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="218" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A218" s="6" t="s">
-        <v>381</v>
+      <c r="A218" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="B218" s="5" t="s">
         <v>544</v>
       </c>
-      <c r="C218" s="6" t="s">
-        <v>382</v>
-      </c>
-      <c r="D218" s="6" t="s">
-        <v>383</v>
-      </c>
-      <c r="E218" s="11" t="s">
-        <v>384</v>
+      <c r="H218" s="13" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="219" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A219" s="6" t="s">
-        <v>386</v>
+      <c r="A219" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="B219" s="5" t="s">
         <v>544</v>
       </c>
-      <c r="C219" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="D219" s="6" t="s">
-        <v>388</v>
-      </c>
-      <c r="E219" s="11" t="s">
-        <v>384</v>
+      <c r="H219" s="13" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="220" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A220" s="6" t="s">
-        <v>393</v>
+      <c r="A220" s="5" t="s">
+        <v>210</v>
       </c>
       <c r="B220" s="5" t="s">
         <v>544</v>
       </c>
-      <c r="C220" s="6" t="s">
-        <v>394</v>
-      </c>
-      <c r="D220" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="E220" s="11" t="s">
-        <v>357</v>
-      </c>
-      <c r="H220" s="13" t="s">
-        <v>520</v>
-      </c>
-      <c r="I220" s="10" t="s">
-        <v>390</v>
-      </c>
     </row>
     <row r="221" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A221" s="6" t="s">
-        <v>396</v>
+      <c r="A221" s="5" t="s">
+        <v>211</v>
       </c>
       <c r="B221" s="5" t="s">
         <v>544</v>
       </c>
-      <c r="C221" s="6" t="s">
-        <v>397</v>
-      </c>
-      <c r="D221" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="E221" s="11" t="s">
-        <v>357</v>
-      </c>
-      <c r="H221" s="13" t="s">
-        <v>520</v>
-      </c>
-      <c r="I221" s="10" t="s">
-        <v>390</v>
-      </c>
     </row>
     <row r="222" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A222" s="6" t="s">
-        <v>398</v>
+      <c r="A222" s="5" t="s">
+        <v>212</v>
       </c>
       <c r="B222" s="5" t="s">
         <v>544</v>
       </c>
-      <c r="C222" s="6" t="s">
-        <v>399</v>
-      </c>
-      <c r="D222" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="E222" s="11" t="s">
-        <v>357</v>
-      </c>
-      <c r="H222" s="13" t="s">
-        <v>520</v>
-      </c>
-      <c r="I222" s="10" t="s">
-        <v>390</v>
-      </c>
     </row>
     <row r="223" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A223" s="6" t="s">
-        <v>413</v>
+      <c r="A223" s="5" t="s">
+        <v>213</v>
       </c>
       <c r="B223" s="5" t="s">
         <v>544</v>
       </c>
-      <c r="C223" s="6" t="s">
+    </row>
+    <row r="224" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A224" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="B224" s="5" t="s">
+        <v>544</v>
+      </c>
+      <c r="C224" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="D224" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="E224" s="11" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A225" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="B225" s="5" t="s">
+        <v>544</v>
+      </c>
+      <c r="C225" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="D225" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="E225" s="11" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A226" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="B226" s="5" t="s">
+        <v>544</v>
+      </c>
+      <c r="C226" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="D226" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="E226" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="H226" s="13" t="s">
+        <v>520</v>
+      </c>
+      <c r="I226" s="10" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A227" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="B227" s="5" t="s">
+        <v>544</v>
+      </c>
+      <c r="C227" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="D227" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="E227" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="H227" s="13" t="s">
+        <v>520</v>
+      </c>
+      <c r="I227" s="10" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="228" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A228" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="B228" s="5" t="s">
+        <v>544</v>
+      </c>
+      <c r="C228" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="D228" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="E228" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="H228" s="13" t="s">
+        <v>520</v>
+      </c>
+      <c r="I228" s="10" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="229" spans="1:9" ht="15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A229" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="B229" s="5" t="s">
+        <v>544</v>
+      </c>
+      <c r="C229" s="6" t="s">
         <v>414</v>
       </c>
-      <c r="D223" s="6" t="s">
+      <c r="D229" s="6" t="s">
         <v>415</v>
       </c>
-      <c r="E223" s="11" t="s">
+      <c r="E229" s="11" t="s">
         <v>357</v>
       </c>
     </row>

</xml_diff>